<commit_message>
objednavky uz mazu udaje z databazy aj pamete
</commit_message>
<xml_diff>
--- a/src/FinalApp/exports/Order.xlsx
+++ b/src/FinalApp/exports/Order.xlsx
@@ -26,16 +26,16 @@
     <t>PNR</t>
   </si>
   <si>
-    <t>Skrina</t>
+    <t>Test material</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>A0002</t>
+    <t>A0001</t>
   </si>
   <si>
-    <t>002</t>
+    <t>2000</t>
   </si>
 </sst>
 </file>

</xml_diff>